<commit_message>
solution book to ggplot2
</commit_message>
<xml_diff>
--- a/tables/books_Hadley.xlsx
+++ b/tables/books_Hadley.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@Quarto projects/Rsources/tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@GitProjects/@2024/rsources-book/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981E6FD5-7322-A948-9915-4DE199FD523E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4375F3-718B-4E42-8657-73619CE87864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14180" xr2:uid="{C0CA3AAC-C072-4A42-94BF-96775068461A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
   <si>
     <t>title</t>
   </si>
@@ -185,6 +185,15 @@
   </si>
   <si>
     <t>https://www.williamspublishing.com/Books/978-5-9909446-8-8.html</t>
+  </si>
+  <si>
+    <t>Aditya Dahiya</t>
+  </si>
+  <si>
+    <t>Solutions Manual (and Beyond) for ggplot2: Elegant Graphics for Data Analysis (3e)</t>
+  </si>
+  <si>
+    <t>https://aditya-dahiya.github.io/ggplot2book3e/</t>
   </si>
 </sst>
 </file>
@@ -540,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5427F2FF-D70F-754B-8DD8-9816C45AB2AF}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -604,211 +613,227 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="1">
+    <row r="4" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>37</v>
+    <row r="8" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>3</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>4</v>
+    <row r="10" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>45</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>38</v>
+      <c r="A12" s="1">
+        <v>5</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>43</v>
+        <v>25</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+    <row r="14" spans="1:5" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>6</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
-        <v>7</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:5" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="17" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="18" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="19" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -824,6 +849,7 @@
     <row r="29" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="30" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="31" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="32" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>